<commit_message>
Waste config file. Regexp tamplates added
</commit_message>
<xml_diff>
--- a/CCICertificate/WebContent/resources/in/WasteNumbers.xlsx
+++ b/CCICertificate/WebContent/resources/in/WasteNumbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20220" windowHeight="12900"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20985" windowHeight="8670"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A36:Q60"/>
 </workbook>
 </file>
 
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>